<commit_message>
possivel escolha  da coluna primaria
</commit_message>
<xml_diff>
--- a/data/func_final.xlsx
+++ b/data/func_final.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -40,18 +40,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
         <bgColor rgb="00FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DE4740"/>
-        <bgColor rgb="00DE4740"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0040DE47"/>
-        <bgColor rgb="0040DE47"/>
       </patternFill>
     </fill>
   </fills>
@@ -73,14 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -446,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,79 +523,86 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>SITUACAO</t>
+          <t>SITUACAO_DATAFRAME</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>PEDRO SILVA</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>FINANÇAS</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>12345678910</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>RUA A</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>JOÃO SILVA</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>MARIA SILVA</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>123</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr"/>
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>BAIRRO X</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>JOÃO PESSOA</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="2" t="inlineStr">
         <is>
           <t>PB</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
         <is>
           <t>12345678</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" s="2" t="inlineStr">
         <is>
           <t>83</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="2" t="inlineStr">
         <is>
           <t>987654321</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr"/>
+      <c r="Q2" s="2" t="inlineStr">
+        <is>
+          <t>ALTERADO</t>
         </is>
       </c>
     </row>
@@ -641,25 +634,17 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>MARIO ANDRÉ</t>
+          <t>CARLOS ALBERTO</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>FERNANDA CARLA</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>456</t>
-        </is>
-      </c>
+          <t>JULIA FERNANDES</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr"/>
       <c r="I3" s="2" t="inlineStr"/>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>BAIRRO X</t>
-        </is>
-      </c>
+      <c r="J3" s="2" t="inlineStr"/>
       <c r="K3" s="2" t="inlineStr">
         <is>
           <t>JOÃO PESSOA</t>
@@ -672,7 +657,7 @@
       </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>54321098</t>
+          <t>59441234</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr">
@@ -682,7 +667,7 @@
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>987654321</t>
+          <t>916221063</t>
         </is>
       </c>
       <c r="P3" s="2" t="inlineStr"/>
@@ -693,29 +678,73 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>LUCAS SANTOS</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>TECNOLOGIA</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>98765432198</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>RUA C</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>CARLOS ALBERTO</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>JULIA FERNANDES</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr"/>
+      <c r="I4" s="2" t="inlineStr"/>
+      <c r="J4" s="2" t="inlineStr"/>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>JOÃO PESSOA</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>59441234</t>
+        </is>
+      </c>
+      <c r="N4" s="2" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>916221063</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr"/>
+      <c r="Q4" s="2" t="inlineStr">
+        <is>
+          <t>ALTERADO</t>
         </is>
       </c>
     </row>
@@ -819,11 +848,7 @@
           <t>87617978563</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>RUA E</t>
-        </is>
-      </c>
+      <c r="E6" s="2" t="inlineStr"/>
       <c r="F6" s="2" t="inlineStr">
         <is>
           <t>CARLOS ALBERTO</t>
@@ -831,20 +856,12 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>JULIA MÊRCEDES</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>1213</t>
-        </is>
-      </c>
+          <t>JULIA FERNANDES</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr"/>
       <c r="I6" s="2" t="inlineStr"/>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>BAIRRO W</t>
-        </is>
-      </c>
+      <c r="J6" s="2" t="inlineStr"/>
       <c r="K6" s="2" t="inlineStr">
         <is>
           <t>JOÃO PESSOA</t>
@@ -857,7 +874,7 @@
       </c>
       <c r="M6" s="2" t="inlineStr">
         <is>
-          <t>67890123</t>
+          <t>59441234</t>
         </is>
       </c>
       <c r="N6" s="2" t="inlineStr">
@@ -913,7 +930,11 @@
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H7" s="2" t="inlineStr"/>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>566</t>
+        </is>
+      </c>
       <c r="I7" s="2" t="inlineStr"/>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -1032,131 +1053,160 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>CAROLINA SOUZA</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>RECURSOS HUMANOS</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>45678912365</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>RUA H</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>PAULO SOUZA</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="2" t="inlineStr">
         <is>
           <t>JULIANA SOUZA</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="2" t="inlineStr">
         <is>
           <t>456</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="I9" s="2" t="inlineStr"/>
+      <c r="J9" s="2" t="inlineStr">
         <is>
           <t>BAIRRO Z</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="K9" s="2" t="inlineStr">
         <is>
           <t>JOÃO PESSOA</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L9" s="2" t="inlineStr">
         <is>
           <t>PB</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="M9" s="2" t="inlineStr">
         <is>
           <t>65432109</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="N9" s="2" t="inlineStr">
         <is>
           <t>83</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="O9" s="2" t="inlineStr">
         <is>
           <t>987654321</t>
+        </is>
+      </c>
+      <c r="P9" s="2" t="inlineStr"/>
+      <c r="Q9" s="2" t="inlineStr">
+        <is>
+          <t>ALTERADO</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>BRUNO ALVES</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>MARKETING</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>85296374100</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>RUA I</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>CARLOS ALBERTO</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>JULIA MÊRCEDES</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>1213</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="inlineStr"/>
+      <c r="J10" s="2" t="inlineStr">
         <is>
           <t>BAIRRO W</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K10" s="2" t="inlineStr">
         <is>
           <t>JOÃO PESSOA</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L10" s="2" t="inlineStr">
         <is>
           <t>PB</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M10" s="2" t="inlineStr">
         <is>
           <t>32109876</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="N10" s="2" t="inlineStr">
         <is>
           <t>83</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="O10" s="2" t="inlineStr">
         <is>
           <t>987654321</t>
+        </is>
+      </c>
+      <c r="P10" s="2" t="inlineStr"/>
+      <c r="Q10" s="2" t="inlineStr">
+        <is>
+          <t>ALTERADO</t>
         </is>
       </c>
     </row>
@@ -1236,289 +1286,278 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>MARCIO JOSÉ</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>RECURSOS HUMANOS</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>50977808264</t>
         </is>
       </c>
-      <c r="E12" s="3" t="inlineStr"/>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr"/>
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>CARLOS ALBERTO</t>
         </is>
       </c>
-      <c r="G12" s="3" t="inlineStr">
+      <c r="G12" s="2" t="inlineStr">
         <is>
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H12" s="3" t="inlineStr"/>
-      <c r="I12" s="3" t="inlineStr"/>
-      <c r="J12" s="3" t="inlineStr"/>
-      <c r="K12" s="3" t="inlineStr">
+      <c r="H12" s="2" t="inlineStr"/>
+      <c r="I12" s="2" t="inlineStr"/>
+      <c r="J12" s="2" t="inlineStr"/>
+      <c r="K12" s="2" t="inlineStr">
         <is>
           <t>JOAO PESSOA</t>
         </is>
       </c>
-      <c r="L12" s="3" t="inlineStr">
+      <c r="L12" s="2" t="inlineStr">
         <is>
           <t>PB</t>
         </is>
       </c>
-      <c r="M12" s="3" t="inlineStr">
+      <c r="M12" s="2" t="inlineStr">
         <is>
           <t>59441234</t>
         </is>
       </c>
-      <c r="N12" s="3" t="inlineStr">
+      <c r="N12" s="2" t="inlineStr">
         <is>
           <t>83</t>
         </is>
       </c>
-      <c r="O12" s="3" t="inlineStr">
+      <c r="O12" s="2" t="inlineStr">
         <is>
           <t>916221063</t>
         </is>
       </c>
-      <c r="P12" s="3" t="inlineStr"/>
-      <c r="Q12" s="3" t="inlineStr">
+      <c r="P12" s="2" t="inlineStr"/>
+      <c r="Q12" s="2" t="inlineStr">
         <is>
           <t>ALTERADO</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>FERNANDA COSTA</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>SUPORTE TÉCNICO</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>36985214700</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>RUA L</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>ANDRÉ COSTA</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="2" t="inlineStr">
         <is>
           <t>CAROLINA COSTA</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="inlineStr"/>
+      <c r="I13" s="2" t="inlineStr"/>
+      <c r="J13" s="2" t="inlineStr"/>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>JOÃO PESSOA</t>
+        </is>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="M13" s="2" t="inlineStr">
+        <is>
+          <t>59441234</t>
+        </is>
+      </c>
+      <c r="N13" s="2" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O13" s="2" t="inlineStr">
+        <is>
+          <t>916221063</t>
+        </is>
+      </c>
+      <c r="P13" s="2" t="inlineStr"/>
+      <c r="Q13" s="2" t="inlineStr">
+        <is>
+          <t>ALTERADO</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>GABRIELA LIMA</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>ATENDIMENTO</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>14725836900</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>RUA N</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t>PEDRO LIMA</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" s="2" t="inlineStr">
         <is>
           <t>MARIA LIMA</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="inlineStr"/>
+      <c r="I14" s="2" t="inlineStr"/>
+      <c r="J14" s="2" t="inlineStr"/>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>JOÃO PESSOA</t>
+        </is>
+      </c>
+      <c r="L14" s="2" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="M14" s="2" t="inlineStr">
+        <is>
+          <t>59441234</t>
+        </is>
+      </c>
+      <c r="N14" s="2" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>916221063</t>
+        </is>
+      </c>
+      <c r="P14" s="2" t="inlineStr"/>
+      <c r="Q14" s="2" t="inlineStr">
+        <is>
+          <t>ALTERADO</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>MARIA CLÁUDIA</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>RECURSOS HUMANOS</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>51147045250</t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr"/>
-      <c r="F15" s="3" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr"/>
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t>CARLOS ALBERTO</t>
         </is>
       </c>
-      <c r="G15" s="3" t="inlineStr">
+      <c r="G15" s="2" t="inlineStr">
         <is>
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H15" s="3" t="inlineStr"/>
-      <c r="I15" s="3" t="inlineStr"/>
-      <c r="J15" s="3" t="inlineStr"/>
-      <c r="K15" s="3" t="inlineStr">
+      <c r="H15" s="2" t="inlineStr"/>
+      <c r="I15" s="2" t="inlineStr"/>
+      <c r="J15" s="2" t="inlineStr"/>
+      <c r="K15" s="2" t="inlineStr">
         <is>
           <t>JOÃO PESSOA</t>
         </is>
       </c>
-      <c r="L15" s="3" t="inlineStr">
+      <c r="L15" s="2" t="inlineStr">
         <is>
           <t>PB</t>
         </is>
       </c>
-      <c r="M15" s="3" t="inlineStr">
-        <is>
-          <t>52210901</t>
-        </is>
-      </c>
-      <c r="N15" s="3" t="inlineStr">
+      <c r="M15" s="2" t="inlineStr">
+        <is>
+          <t>59441234</t>
+        </is>
+      </c>
+      <c r="N15" s="2" t="inlineStr">
         <is>
           <t>83</t>
         </is>
       </c>
-      <c r="O15" s="3" t="inlineStr">
+      <c r="O15" s="2" t="inlineStr">
         <is>
           <t>931857921</t>
         </is>
       </c>
-      <c r="P15" s="3" t="inlineStr"/>
-      <c r="Q15" s="3" t="inlineStr">
+      <c r="P15" s="2" t="inlineStr"/>
+      <c r="Q15" s="2" t="inlineStr">
         <is>
           <t>ALTERADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>MARIA LUIZA</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>SUPORTE TÉCNICO</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="inlineStr">
-        <is>
-          <t>94585301234</t>
-        </is>
-      </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>RUA J</t>
-        </is>
-      </c>
-      <c r="F16" s="4" t="inlineStr">
-        <is>
-          <t>CARLOS ALBERTO</t>
-        </is>
-      </c>
-      <c r="G16" s="4" t="inlineStr">
-        <is>
-          <t>JULIA FERNANDES</t>
-        </is>
-      </c>
-      <c r="H16" s="4" t="inlineStr">
-        <is>
-          <t>566</t>
-        </is>
-      </c>
-      <c r="I16" s="4" t="inlineStr"/>
-      <c r="J16" s="4" t="inlineStr">
-        <is>
-          <t>BAIRRO A</t>
-        </is>
-      </c>
-      <c r="K16" s="4" t="inlineStr">
-        <is>
-          <t>JOÃO PESSOA</t>
-        </is>
-      </c>
-      <c r="L16" s="4" t="inlineStr">
-        <is>
-          <t>PB</t>
-        </is>
-      </c>
-      <c r="M16" s="4" t="inlineStr">
-        <is>
-          <t>52210901</t>
-        </is>
-      </c>
-      <c r="N16" s="4" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
-      </c>
-      <c r="O16" s="4" t="inlineStr">
-        <is>
-          <t>935859334</t>
-        </is>
-      </c>
-      <c r="P16" s="4" t="inlineStr"/>
-      <c r="Q16" s="4" t="inlineStr">
-        <is>
-          <t>ADICIONADO</t>
         </is>
       </c>
     </row>

</xml_diff>